<commit_message>
Added wind columns for analysis
</commit_message>
<xml_diff>
--- a/Data/Power/Node/2020-06-06--.xlsx
+++ b/Data/Power/Node/2020-06-06--.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriann Liceralde\Desktop\Repository\WirelessSensorNetwork\Data\Power\Node\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Desktop\Repository\WirelessSensorNetwork\Data\Power\Node\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1410252D-E0FB-47BA-877A-182444241919}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8AC1F4F-069C-4BCE-9BD5-41B6DDF50AED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10898" yWindow="3855" windowWidth="15390" windowHeight="9533" xr2:uid="{837BAD77-3217-40E5-A7E4-660EDC5FE3AD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{837BAD77-3217-40E5-A7E4-660EDC5FE3AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -194,6 +194,98 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="62"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-ABCE-423B-AB60-8DF0434794B4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="454"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.3333333333333332E-3"/>
+                  <c:y val="-2.7777777777777776E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-ABCE-423B-AB60-8DF0434794B4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$C$37:$C$1091</c:f>
@@ -9417,7 +9509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DAC104-C7D0-4643-921E-A90CC36D0D4D}">
   <dimension ref="A1:H1091"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -24758,12 +24850,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100985DCE29A6F5F4498900247CF69BBF1C" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5a912827122eb319b0c882e54fe6e373">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f16e2849-3890-4a49-a752-654daf59a737" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a4084dc4b0e9a9611e3657dcb164be4c" ns3:_="">
     <xsd:import namespace="f16e2849-3890-4a49-a752-654daf59a737"/>
@@ -24947,6 +25033,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -24957,22 +25049,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85ABC463-26A8-4942-A14D-D127B9F23005}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="f16e2849-3890-4a49-a752-654daf59a737"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C286A821-AC86-4064-99FA-4BA05E87EAE6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24990,6 +25066,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85ABC463-26A8-4942-A14D-D127B9F23005}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="f16e2849-3890-4a49-a752-654daf59a737"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F21376D-7705-4268-9809-DADD2814B81D}">
   <ds:schemaRefs>

</xml_diff>